<commit_message>
Added the new merged Version with Zane's Solid Machine and with Fill Flash
</commit_message>
<xml_diff>
--- a/ShutterSpeeds (version 1).xlsx
+++ b/ShutterSpeeds (version 1).xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Uni Frankfurt\OneDrive - stud.uni-frankfurt.de\Fotografie\OpenSX-70\Oktober\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="526" documentId="8_{94177CF9-B5A9-45DA-9C08-ABB210FBC242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8463BD19-C517-4B3E-BEFF-B795ECBFFF53}"/>
+  <xr:revisionPtr revIDLastSave="710" documentId="8_{94177CF9-B5A9-45DA-9C08-ABB210FBC242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F91B3077-BAC3-4576-961D-27D8783EF8B3}"/>
   <bookViews>
-    <workbookView xWindow="9375" yWindow="120" windowWidth="10395" windowHeight="10725" activeTab="1" xr2:uid="{8179858F-0FCB-4BE4-82F9-54BAD174FD57}"/>
+    <workbookView minimized="1" xWindow="13485" yWindow="930" windowWidth="10395" windowHeight="10725" firstSheet="2" activeTab="3" xr2:uid="{8179858F-0FCB-4BE4-82F9-54BAD174FD57}"/>
   </bookViews>
   <sheets>
     <sheet name="TCS3200-AlphaModel2" sheetId="1" r:id="rId1"/>
     <sheet name="TCS3200 Deault" sheetId="3" r:id="rId2"/>
-    <sheet name="Alpha-Edwin_TSL327" sheetId="4" r:id="rId3"/>
-    <sheet name="TSL327T-Alpha" sheetId="2" r:id="rId4"/>
+    <sheet name="Tabelle1" sheetId="5" r:id="rId3"/>
+    <sheet name="Alpha-Edwin_TSL327" sheetId="4" r:id="rId4"/>
+    <sheet name="TCS3200-Sonar Black Measurement" sheetId="6" r:id="rId5"/>
+    <sheet name="TSL327T-Alpha" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="51">
   <si>
     <t>Edwin</t>
   </si>
@@ -171,18 +173,37 @@
   </si>
   <si>
     <t>25, 29, 32, 34, 39, 44, 54, 87, 175, 311, 609, 1109</t>
+  </si>
+  <si>
+    <t>0.9, 1.64, 3.22, 5.71, 11.49, 18.52, 22.73, 25.64, 29.41, 31.25, 34.48, 40</t>
+  </si>
+  <si>
+    <t>1/4 CCW</t>
+  </si>
+  <si>
+    <t>1/2 CCW</t>
+  </si>
+  <si>
+    <t>2/3 CCW</t>
+  </si>
+  <si>
+    <t>1/1 CCW</t>
+  </si>
+  <si>
+    <t>Wieder auf Std</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +213,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -287,10 +315,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -321,8 +350,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -637,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6512B97-FAD2-4678-B2F2-D5662BC4FA52}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,20 +1461,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D28D8C7-2D72-4878-89D7-B6CFC4BF87E8}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +1488,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1470,14 +1502,14 @@
         <f>C3/C2</f>
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1489,7 +1521,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8" t="s">
         <v>25</v>
@@ -1504,47 +1536,48 @@
         <v>23</v>
       </c>
       <c r="F5" s="8"/>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="J5" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="K5" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="L5" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="M5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="N5" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="O5" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="P5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="Q5" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="R5" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="R5" s="16" t="s">
+      <c r="S5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -1560,62 +1593,66 @@
         <v>16</v>
       </c>
       <c r="E6" s="7">
-        <f>D6+$H$2</f>
+        <f>D6+$I$2</f>
         <v>25</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
+        <f>1/E6*1000</f>
+        <v>40</v>
+      </c>
+      <c r="H6">
         <v>2000</v>
       </c>
-      <c r="H6" s="11">
-        <f>1/G6</f>
+      <c r="I6" s="11">
+        <f>1/H6</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="I6" s="3">
-        <f>H6*1000</f>
+      <c r="J6" s="3">
+        <f>I6*1000</f>
         <v>0.5</v>
       </c>
-      <c r="J6" s="3">
-        <f>E6-I6</f>
+      <c r="K6" s="3">
+        <f t="shared" ref="K6:K17" si="0">E6-J6</f>
         <v>24.5</v>
       </c>
-      <c r="K6" s="12">
+      <c r="L6" s="12">
         <v>57.3</v>
       </c>
-      <c r="L6" s="1">
-        <f>LOG(((K6^2)/N6),2)</f>
+      <c r="M6" s="1">
+        <f>LOG(((L6^2)/O6),2)</f>
         <v>17</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>17</v>
       </c>
-      <c r="N6" s="24">
-        <f>2^-M6*K6^2</f>
+      <c r="O6" s="24">
+        <f>2^-N6*L6^2</f>
         <v>2.5049514770507809E-2</v>
       </c>
-      <c r="O6" s="17">
-        <f>N6*1000</f>
+      <c r="P6" s="17">
+        <f>O6*1000</f>
         <v>25.049514770507809</v>
       </c>
-      <c r="P6" s="1">
-        <f>O6</f>
+      <c r="Q6" s="1">
+        <f>P6</f>
         <v>25.049514770507809</v>
       </c>
-      <c r="Q6" s="1">
-        <f>P6-$H$2</f>
+      <c r="R6" s="1">
+        <f>Q6-$I$2</f>
         <v>16.049514770507809</v>
       </c>
-      <c r="R6">
-        <f t="shared" ref="R6:R17" si="0">E6/I6</f>
+      <c r="S6">
+        <f t="shared" ref="S6:S17" si="1">E6/J6</f>
         <v>50</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
@@ -1623,70 +1660,74 @@
         <v>20</v>
       </c>
       <c r="C7" s="7">
-        <f t="shared" ref="C7:C17" si="1">B7*$E$2</f>
+        <f t="shared" ref="C7:C17" si="2">B7*$E$2</f>
         <v>20</v>
       </c>
       <c r="D7" s="7">
-        <f t="shared" ref="D7:D17" si="2">C7</f>
+        <f t="shared" ref="D7:D17" si="3">C7</f>
         <v>20</v>
       </c>
       <c r="E7" s="7">
-        <f t="shared" ref="E7:E17" si="3">D7+$H$2</f>
+        <f t="shared" ref="E7:E17" si="4">D7+$I$2</f>
         <v>29</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
+        <f t="shared" ref="G7:G16" si="5">1/E7*1000</f>
+        <v>34.482758620689651</v>
+      </c>
+      <c r="H7">
         <v>1000</v>
       </c>
-      <c r="H7" s="11">
-        <f t="shared" ref="H7:H17" si="4">1/G7</f>
+      <c r="I7" s="11">
+        <f t="shared" ref="I7:I17" si="6">1/H7</f>
         <v>1E-3</v>
       </c>
-      <c r="I7" s="3">
-        <f t="shared" ref="I7:I17" si="5">H7*1000</f>
+      <c r="J7" s="3">
+        <f t="shared" ref="J7:J17" si="7">I7*1000</f>
         <v>1</v>
       </c>
-      <c r="J7" s="3">
-        <f t="shared" ref="J7:J17" si="6">E7-I7</f>
+      <c r="K7" s="3">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="K7" s="12">
+      <c r="L7" s="12">
         <v>43.8</v>
       </c>
-      <c r="L7" s="1">
-        <f t="shared" ref="L7:L17" si="7">LOG(((K7^2)/N7),2)</f>
+      <c r="M7" s="1">
+        <f t="shared" ref="M7:M17" si="8">LOG(((L7^2)/O7),2)</f>
         <v>16</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>16</v>
       </c>
-      <c r="N7" s="24">
-        <f t="shared" ref="N7:N17" si="8">2^-M7*K7^2</f>
+      <c r="O7" s="24">
+        <f t="shared" ref="O7:O17" si="9">2^-N7*L7^2</f>
         <v>2.9273071289062497E-2</v>
       </c>
-      <c r="O7" s="17">
-        <f t="shared" ref="O7:O17" si="9">N7*1000</f>
+      <c r="P7" s="17">
+        <f t="shared" ref="P7:P17" si="10">O7*1000</f>
         <v>29.273071289062496</v>
       </c>
-      <c r="P7" s="1">
-        <f t="shared" ref="P7:P17" si="10">O7</f>
+      <c r="Q7" s="1">
+        <f t="shared" ref="Q7:Q17" si="11">P7</f>
         <v>29.273071289062496</v>
       </c>
-      <c r="Q7" s="1">
-        <f t="shared" ref="Q7:Q17" si="11">P7-$H$2</f>
+      <c r="R7" s="1">
+        <f t="shared" ref="R7:R17" si="12">Q7-$I$2</f>
         <v>20.273071289062496</v>
       </c>
-      <c r="R7">
-        <f t="shared" si="0"/>
+      <c r="S7">
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -1694,67 +1735,71 @@
         <v>23</v>
       </c>
       <c r="C8" s="7">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="D8" s="7">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
+      <c r="D8" s="7">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
       <c r="E8" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
+        <f t="shared" si="5"/>
+        <v>31.25</v>
+      </c>
+      <c r="H8">
         <v>500</v>
       </c>
-      <c r="H8" s="11">
-        <f t="shared" si="4"/>
+      <c r="I8" s="11">
+        <f t="shared" si="6"/>
         <v>2E-3</v>
       </c>
-      <c r="I8" s="3">
-        <f t="shared" si="5"/>
+      <c r="J8" s="3">
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="J8" s="3">
-        <f t="shared" si="6"/>
+      <c r="K8" s="3">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K8" s="12">
+      <c r="L8" s="12">
         <v>32.4</v>
       </c>
-      <c r="L8" s="1">
-        <f t="shared" si="7"/>
+      <c r="M8" s="1">
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>15</v>
       </c>
-      <c r="N8" s="24">
-        <f t="shared" si="8"/>
+      <c r="O8" s="24">
+        <f t="shared" si="9"/>
         <v>3.20361328125E-2</v>
       </c>
-      <c r="O8" s="17">
-        <f t="shared" si="9"/>
-        <v>32.0361328125</v>
-      </c>
-      <c r="P8" s="1">
+      <c r="P8" s="17">
         <f t="shared" si="10"/>
         <v>32.0361328125</v>
       </c>
       <c r="Q8" s="1">
         <f t="shared" si="11"/>
+        <v>32.0361328125</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="12"/>
         <v>23.0361328125</v>
       </c>
-      <c r="R8">
-        <f t="shared" si="0"/>
+      <c r="S8">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -1762,67 +1807,71 @@
         <v>25</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="D9" s="7">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
+      <c r="D9" s="7">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
       <c r="E9" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
+        <f t="shared" si="5"/>
+        <v>29.411764705882351</v>
+      </c>
+      <c r="H9">
         <v>250</v>
       </c>
-      <c r="H9" s="11">
-        <f t="shared" si="4"/>
+      <c r="I9" s="11">
+        <f t="shared" si="6"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I9" s="3">
-        <f t="shared" si="5"/>
+      <c r="J9" s="3">
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="J9" s="3">
-        <f t="shared" si="6"/>
+      <c r="K9" s="3">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K9" s="12">
+      <c r="L9" s="12">
         <v>23.6</v>
       </c>
-      <c r="L9" s="1">
-        <f t="shared" si="7"/>
+      <c r="M9" s="1">
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>14</v>
       </c>
-      <c r="N9" s="24">
-        <f t="shared" si="8"/>
+      <c r="O9" s="24">
+        <f t="shared" si="9"/>
         <v>3.3994140625000002E-2</v>
       </c>
-      <c r="O9" s="17">
-        <f t="shared" si="9"/>
-        <v>33.994140625</v>
-      </c>
-      <c r="P9" s="1">
+      <c r="P9" s="17">
         <f t="shared" si="10"/>
         <v>33.994140625</v>
       </c>
       <c r="Q9" s="1">
         <f t="shared" si="11"/>
+        <v>33.994140625</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="12"/>
         <v>24.994140625</v>
       </c>
-      <c r="R9">
-        <f t="shared" si="0"/>
+      <c r="S9">
+        <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -1830,67 +1879,71 @@
         <v>30</v>
       </c>
       <c r="C10" s="7">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="D10" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
+      <c r="D10" s="7">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
       <c r="E10" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
+        <f t="shared" si="5"/>
+        <v>25.641025641025639</v>
+      </c>
+      <c r="H10">
         <v>125</v>
       </c>
-      <c r="H10" s="11">
-        <f t="shared" si="4"/>
+      <c r="I10" s="11">
+        <f t="shared" si="6"/>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I10" s="3">
-        <f t="shared" si="5"/>
+      <c r="J10" s="3">
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="J10" s="3">
-        <f t="shared" si="6"/>
+      <c r="K10" s="3">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="K10" s="12">
+      <c r="L10" s="12">
         <v>17.64</v>
       </c>
-      <c r="L10" s="1">
-        <f t="shared" si="7"/>
+      <c r="M10" s="1">
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>13</v>
       </c>
-      <c r="N10" s="24">
-        <f t="shared" si="8"/>
+      <c r="O10" s="24">
+        <f t="shared" si="9"/>
         <v>3.79845703125E-2</v>
       </c>
-      <c r="O10" s="17">
-        <f t="shared" si="9"/>
-        <v>37.984570312499997</v>
-      </c>
-      <c r="P10" s="1">
+      <c r="P10" s="17">
         <f t="shared" si="10"/>
         <v>37.984570312499997</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="11"/>
+        <v>37.984570312499997</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" si="12"/>
         <v>28.984570312499997</v>
       </c>
-      <c r="R10">
-        <f t="shared" si="0"/>
+      <c r="S10">
+        <f t="shared" si="1"/>
         <v>4.875</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
@@ -1898,67 +1951,71 @@
         <v>35</v>
       </c>
       <c r="C11" s="7">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="D11" s="7">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
+      <c r="D11" s="7">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
       <c r="E11" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
+        <f t="shared" si="5"/>
+        <v>22.727272727272727</v>
+      </c>
+      <c r="H11">
         <v>60</v>
       </c>
-      <c r="H11" s="11">
-        <f t="shared" si="4"/>
+      <c r="I11" s="11">
+        <f t="shared" si="6"/>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="I11" s="3">
-        <f t="shared" si="5"/>
+      <c r="J11" s="3">
+        <f t="shared" si="7"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="J11" s="3">
-        <f t="shared" si="6"/>
+      <c r="K11" s="3">
+        <f t="shared" si="0"/>
         <v>27.333333333333332</v>
       </c>
-      <c r="K11" s="12">
+      <c r="L11" s="12">
         <v>13.42</v>
       </c>
-      <c r="L11" s="1">
-        <f t="shared" si="7"/>
+      <c r="M11" s="1">
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>12</v>
       </c>
-      <c r="N11" s="24">
-        <f t="shared" si="8"/>
+      <c r="O11" s="24">
+        <f t="shared" si="9"/>
         <v>4.3968847656249997E-2</v>
       </c>
-      <c r="O11" s="17">
-        <f t="shared" si="9"/>
-        <v>43.968847656249999</v>
-      </c>
-      <c r="P11" s="1">
+      <c r="P11" s="17">
         <f t="shared" si="10"/>
         <v>43.968847656249999</v>
       </c>
       <c r="Q11" s="1">
         <f t="shared" si="11"/>
+        <v>43.968847656249999</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="12"/>
         <v>34.968847656249999</v>
       </c>
-      <c r="R11">
-        <f t="shared" si="0"/>
+      <c r="S11">
+        <f t="shared" si="1"/>
         <v>2.6399999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
@@ -1966,67 +2023,71 @@
         <v>45</v>
       </c>
       <c r="C12" s="7">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="D12" s="7">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
+      <c r="D12" s="7">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
       <c r="E12" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
+        <f t="shared" si="5"/>
+        <v>18.518518518518519</v>
+      </c>
+      <c r="H12">
         <v>30</v>
       </c>
-      <c r="H12" s="11">
-        <f t="shared" si="4"/>
+      <c r="I12" s="11">
+        <f t="shared" si="6"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="I12" s="3">
-        <f t="shared" si="5"/>
+      <c r="J12" s="3">
+        <f t="shared" si="7"/>
         <v>33.333333333333336</v>
       </c>
-      <c r="J12" s="3">
-        <f t="shared" si="6"/>
+      <c r="K12" s="3">
+        <f t="shared" si="0"/>
         <v>20.666666666666664</v>
       </c>
-      <c r="K12" s="12">
+      <c r="L12" s="12">
         <v>10.5</v>
       </c>
-      <c r="L12" s="1">
-        <f t="shared" si="7"/>
+      <c r="M12" s="1">
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>11</v>
       </c>
-      <c r="N12" s="24">
-        <f t="shared" si="8"/>
+      <c r="O12" s="24">
+        <f t="shared" si="9"/>
         <v>5.38330078125E-2</v>
       </c>
-      <c r="O12" s="17">
-        <f t="shared" si="9"/>
-        <v>53.8330078125</v>
-      </c>
-      <c r="P12" s="1">
+      <c r="P12" s="17">
         <f t="shared" si="10"/>
         <v>53.8330078125</v>
       </c>
       <c r="Q12" s="1">
         <f t="shared" si="11"/>
+        <v>53.8330078125</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="12"/>
         <v>44.8330078125</v>
       </c>
-      <c r="R12">
-        <f t="shared" si="0"/>
+      <c r="S12">
+        <f t="shared" si="1"/>
         <v>1.6199999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>14</v>
       </c>
@@ -2038,63 +2099,67 @@
         <v>78</v>
       </c>
       <c r="D13" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>78</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
+        <f t="shared" si="5"/>
+        <v>11.494252873563218</v>
+      </c>
+      <c r="H13">
         <v>15</v>
       </c>
-      <c r="H13" s="11">
-        <f t="shared" si="4"/>
+      <c r="I13" s="11">
+        <f t="shared" si="6"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="I13" s="3">
-        <f t="shared" si="5"/>
+      <c r="J13" s="3">
+        <f t="shared" si="7"/>
         <v>66.666666666666671</v>
       </c>
-      <c r="J13" s="3">
-        <f t="shared" si="6"/>
+      <c r="K13" s="3">
+        <f t="shared" si="0"/>
         <v>20.333333333333329</v>
       </c>
-      <c r="K13" s="12">
+      <c r="L13" s="12">
         <v>9.44</v>
       </c>
-      <c r="L13" s="1">
-        <f t="shared" si="7"/>
+      <c r="M13" s="1">
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>10</v>
       </c>
-      <c r="N13" s="24">
-        <f t="shared" si="8"/>
+      <c r="O13" s="24">
+        <f t="shared" si="9"/>
         <v>8.7024999999999991E-2</v>
       </c>
-      <c r="O13" s="17">
-        <f t="shared" si="9"/>
-        <v>87.024999999999991</v>
-      </c>
-      <c r="P13" s="1">
+      <c r="P13" s="17">
         <f t="shared" si="10"/>
         <v>87.024999999999991</v>
       </c>
       <c r="Q13" s="1">
         <f t="shared" si="11"/>
+        <v>87.024999999999991</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="12"/>
         <v>78.024999999999991</v>
       </c>
-      <c r="R13">
-        <f t="shared" si="0"/>
+      <c r="S13">
+        <f t="shared" si="1"/>
         <v>1.3049999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
@@ -2102,67 +2167,71 @@
         <v>166</v>
       </c>
       <c r="C14" s="7">
-        <f t="shared" si="1"/>
-        <v>166</v>
-      </c>
-      <c r="D14" s="7">
         <f t="shared" si="2"/>
         <v>166</v>
       </c>
+      <c r="D14" s="7">
+        <f t="shared" si="3"/>
+        <v>166</v>
+      </c>
       <c r="E14" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>175</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
+        <f t="shared" si="5"/>
+        <v>5.7142857142857144</v>
+      </c>
+      <c r="H14">
         <v>8</v>
       </c>
-      <c r="H14" s="11">
-        <f t="shared" si="4"/>
+      <c r="I14" s="11">
+        <f t="shared" si="6"/>
         <v>0.125</v>
       </c>
-      <c r="I14" s="3">
-        <f t="shared" si="5"/>
+      <c r="J14" s="3">
+        <f t="shared" si="7"/>
         <v>125</v>
       </c>
-      <c r="J14" s="3">
-        <f t="shared" si="6"/>
+      <c r="K14" s="3">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="K14" s="12">
+      <c r="L14" s="12">
         <v>9.4670000000000005</v>
       </c>
-      <c r="L14" s="1">
-        <f t="shared" si="7"/>
+      <c r="M14" s="1">
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>9</v>
       </c>
-      <c r="N14" s="24">
-        <f t="shared" si="8"/>
+      <c r="O14" s="24">
+        <f t="shared" si="9"/>
         <v>0.17504704882812502</v>
       </c>
-      <c r="O14" s="17">
-        <f t="shared" si="9"/>
-        <v>175.04704882812501</v>
-      </c>
-      <c r="P14" s="1">
+      <c r="P14" s="17">
         <f t="shared" si="10"/>
         <v>175.04704882812501</v>
       </c>
       <c r="Q14" s="1">
         <f t="shared" si="11"/>
+        <v>175.04704882812501</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="12"/>
         <v>166.04704882812501</v>
       </c>
-      <c r="R14">
-        <f t="shared" si="0"/>
+      <c r="S14">
+        <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
@@ -2170,67 +2239,71 @@
         <v>302</v>
       </c>
       <c r="C15" s="7">
-        <f t="shared" si="1"/>
-        <v>302</v>
-      </c>
-      <c r="D15" s="7">
         <f t="shared" si="2"/>
         <v>302</v>
       </c>
+      <c r="D15" s="7">
+        <f t="shared" si="3"/>
+        <v>302</v>
+      </c>
       <c r="E15" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>311</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
+        <f t="shared" si="5"/>
+        <v>3.215434083601286</v>
+      </c>
+      <c r="H15">
         <v>4</v>
       </c>
-      <c r="H15" s="11">
-        <f t="shared" si="4"/>
+      <c r="I15" s="11">
+        <f t="shared" si="6"/>
         <v>0.25</v>
       </c>
-      <c r="I15" s="3">
-        <f t="shared" si="5"/>
+      <c r="J15" s="3">
+        <f t="shared" si="7"/>
         <v>250</v>
       </c>
-      <c r="J15" s="3">
-        <f t="shared" si="6"/>
+      <c r="K15" s="3">
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="K15" s="12">
+      <c r="L15" s="12">
         <v>8.9239999999999995</v>
       </c>
-      <c r="L15" s="1">
-        <f t="shared" si="7"/>
+      <c r="M15" s="1">
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>8</v>
       </c>
-      <c r="N15" s="24">
-        <f t="shared" si="8"/>
+      <c r="O15" s="24">
+        <f t="shared" si="9"/>
         <v>0.31108506249999995</v>
       </c>
-      <c r="O15" s="17">
-        <f t="shared" si="9"/>
-        <v>311.08506249999994</v>
-      </c>
-      <c r="P15" s="1">
+      <c r="P15" s="17">
         <f t="shared" si="10"/>
         <v>311.08506249999994</v>
       </c>
       <c r="Q15" s="1">
         <f t="shared" si="11"/>
+        <v>311.08506249999994</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="12"/>
         <v>302.08506249999994</v>
       </c>
-      <c r="R15">
-        <f t="shared" si="0"/>
+      <c r="S15">
+        <f t="shared" si="1"/>
         <v>1.244</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>17</v>
       </c>
@@ -2238,67 +2311,71 @@
         <v>600</v>
       </c>
       <c r="C16" s="7">
-        <f t="shared" si="1"/>
-        <v>600</v>
-      </c>
-      <c r="D16" s="7">
         <f t="shared" si="2"/>
         <v>600</v>
       </c>
+      <c r="D16" s="7">
+        <f t="shared" si="3"/>
+        <v>600</v>
+      </c>
       <c r="E16" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>609</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
+        <f t="shared" si="5"/>
+        <v>1.6420361247947455</v>
+      </c>
+      <c r="H16">
         <v>2</v>
       </c>
-      <c r="H16" s="11">
-        <f t="shared" si="4"/>
+      <c r="I16" s="11">
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="I16" s="3">
-        <f t="shared" si="5"/>
+      <c r="J16" s="3">
+        <f t="shared" si="7"/>
         <v>500</v>
       </c>
-      <c r="J16" s="3">
-        <f t="shared" si="6"/>
+      <c r="K16" s="3">
+        <f t="shared" si="0"/>
         <v>109</v>
       </c>
-      <c r="K16" s="12">
+      <c r="L16" s="12">
         <v>8.83</v>
       </c>
-      <c r="L16" s="1">
-        <f t="shared" si="7"/>
+      <c r="M16" s="1">
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>7</v>
       </c>
-      <c r="N16" s="24">
-        <f t="shared" si="8"/>
+      <c r="O16" s="24">
+        <f t="shared" si="9"/>
         <v>0.60913203125000004</v>
       </c>
-      <c r="O16" s="17">
-        <f t="shared" si="9"/>
-        <v>609.13203125000007</v>
-      </c>
-      <c r="P16" s="1">
+      <c r="P16" s="17">
         <f t="shared" si="10"/>
         <v>609.13203125000007</v>
       </c>
       <c r="Q16" s="1">
         <f t="shared" si="11"/>
+        <v>609.13203125000007</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" si="12"/>
         <v>600.13203125000007</v>
       </c>
-      <c r="R16">
-        <f t="shared" si="0"/>
+      <c r="S16">
+        <f t="shared" si="1"/>
         <v>1.218</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
@@ -2306,74 +2383,83 @@
         <v>1100</v>
       </c>
       <c r="C17" s="7">
-        <f t="shared" si="1"/>
-        <v>1100</v>
-      </c>
-      <c r="D17" s="7">
         <f t="shared" si="2"/>
         <v>1100</v>
       </c>
+      <c r="D17" s="7">
+        <f t="shared" si="3"/>
+        <v>1100</v>
+      </c>
       <c r="E17" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1109</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
+        <f>1/E17*1000</f>
+        <v>0.90171325518485113</v>
+      </c>
+      <c r="H17">
         <v>1</v>
       </c>
-      <c r="H17" s="11">
-        <f t="shared" si="4"/>
+      <c r="I17" s="11">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="I17" s="3">
-        <f t="shared" si="5"/>
+      <c r="J17" s="3">
+        <f t="shared" si="7"/>
         <v>1000</v>
       </c>
-      <c r="J17" s="3">
-        <f t="shared" si="6"/>
+      <c r="K17" s="3">
+        <f t="shared" si="0"/>
         <v>109</v>
       </c>
-      <c r="K17" s="12">
+      <c r="L17" s="12">
         <v>8.4250000000000007</v>
       </c>
-      <c r="L17" s="1">
-        <f t="shared" si="7"/>
+      <c r="M17" s="1">
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>6</v>
       </c>
-      <c r="N17" s="24">
-        <f t="shared" si="8"/>
+      <c r="O17" s="24">
+        <f t="shared" si="9"/>
         <v>1.1090722656250003</v>
       </c>
-      <c r="O17" s="17">
-        <f t="shared" si="9"/>
-        <v>1109.0722656250002</v>
-      </c>
-      <c r="P17" s="1">
+      <c r="P17" s="17">
         <f t="shared" si="10"/>
         <v>1109.0722656250002</v>
       </c>
       <c r="Q17" s="1">
         <f t="shared" si="11"/>
+        <v>1109.0722656250002</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="12"/>
         <v>1100.0722656250002</v>
       </c>
-      <c r="R17">
-        <f t="shared" si="0"/>
+      <c r="S17">
+        <f t="shared" si="1"/>
         <v>1.109</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2383,11 +2469,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D332B89-108B-4268-B1E5-C721524C3137}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9DD51A-1A45-4D0D-AB97-C59113CA7CB4}">
   <dimension ref="A1:AM15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2563,6 +2661,9 @@
       <c r="R4">
         <v>41</v>
       </c>
+      <c r="AM4">
+        <v>1.1200000000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -2605,6 +2706,9 @@
       <c r="R5">
         <v>43</v>
       </c>
+      <c r="AM5">
+        <v>1.1200000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -2623,6 +2727,9 @@
       <c r="F6">
         <v>27</v>
       </c>
+      <c r="I6">
+        <v>32</v>
+      </c>
       <c r="K6">
         <v>50</v>
       </c>
@@ -2640,6 +2747,9 @@
       </c>
       <c r="R6">
         <v>42</v>
+      </c>
+      <c r="AM6">
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
@@ -2659,11 +2769,17 @@
       <c r="F7">
         <v>29</v>
       </c>
+      <c r="I7">
+        <v>32</v>
+      </c>
       <c r="K7">
         <v>49</v>
       </c>
       <c r="L7">
         <v>35</v>
+      </c>
+      <c r="O7">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
@@ -2677,6 +2793,18 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
+      <c r="F8">
+        <v>27</v>
+      </c>
+      <c r="I8">
+        <v>33</v>
+      </c>
+      <c r="L8">
+        <v>34</v>
+      </c>
+      <c r="O8">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -2689,6 +2817,12 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
+      <c r="F9">
+        <v>28</v>
+      </c>
+      <c r="O9">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -2701,6 +2835,12 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
+      <c r="F10">
+        <v>27</v>
+      </c>
+      <c r="O10">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -2713,6 +2853,9 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
+      <c r="F11">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -2725,6 +2868,15 @@
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
+      <c r="F12">
+        <v>24</v>
+      </c>
+      <c r="I12">
+        <v>23</v>
+      </c>
+      <c r="L12">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -2736,6 +2888,12 @@
       <c r="C13" s="7">
         <f t="shared" si="0"/>
         <v>311</v>
+      </c>
+      <c r="I13">
+        <v>23</v>
+      </c>
+      <c r="L13">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
@@ -2767,7 +2925,620 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02013D2-9898-4BC7-90A9-2AA01E6C5832}">
+  <dimension ref="A1:AM47"/>
+  <sheetViews>
+    <sheetView topLeftCell="M28" workbookViewId="0">
+      <selection activeCell="R48" sqref="R48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="W3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="10">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7">
+        <f t="shared" ref="C4:C15" si="0">B4+$B$2</f>
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>31</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="K4">
+        <v>33</v>
+      </c>
+      <c r="L4">
+        <v>17</v>
+      </c>
+      <c r="N4">
+        <v>35</v>
+      </c>
+      <c r="O4">
+        <v>20</v>
+      </c>
+      <c r="R4">
+        <v>27</v>
+      </c>
+      <c r="S4">
+        <v>45</v>
+      </c>
+      <c r="U4">
+        <v>32</v>
+      </c>
+      <c r="AM4">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>26</v>
+      </c>
+      <c r="F5" s="26">
+        <v>9.34</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5">
+        <v>16</v>
+      </c>
+      <c r="K5">
+        <v>33</v>
+      </c>
+      <c r="L5">
+        <v>14</v>
+      </c>
+      <c r="N5">
+        <v>35</v>
+      </c>
+      <c r="O5">
+        <v>18</v>
+      </c>
+      <c r="R5">
+        <v>28</v>
+      </c>
+      <c r="S5">
+        <v>45</v>
+      </c>
+      <c r="U5">
+        <v>33</v>
+      </c>
+      <c r="AM5">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="10">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <v>8.77</v>
+      </c>
+      <c r="H6">
+        <v>31</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="K6">
+        <v>34</v>
+      </c>
+      <c r="L6">
+        <v>16</v>
+      </c>
+      <c r="N6">
+        <v>35</v>
+      </c>
+      <c r="O6">
+        <v>20</v>
+      </c>
+      <c r="S6">
+        <v>45</v>
+      </c>
+      <c r="U6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="10">
+        <v>25</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E7">
+        <v>27</v>
+      </c>
+      <c r="F7">
+        <v>8.69</v>
+      </c>
+      <c r="H7">
+        <v>31</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="N7">
+        <v>35</v>
+      </c>
+      <c r="O7">
+        <v>23</v>
+      </c>
+      <c r="S7">
+        <v>45</v>
+      </c>
+      <c r="U7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10">
+        <v>30</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="H8">
+        <v>31</v>
+      </c>
+      <c r="I8">
+        <v>8.86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="10">
+        <v>35</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="I9">
+        <v>9.66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="10">
+        <v>45</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="10">
+        <v>55</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="10">
+        <v>166</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="10">
+        <v>302</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="10">
+        <v>600</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="0"/>
+        <v>609</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="10">
+        <v>1100</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="0"/>
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19">
+        <v>27</v>
+      </c>
+      <c r="F19">
+        <v>16</v>
+      </c>
+      <c r="H19">
+        <v>31</v>
+      </c>
+      <c r="I19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>16</v>
+      </c>
+      <c r="I22">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23">
+        <v>27</v>
+      </c>
+      <c r="F23">
+        <v>20</v>
+      </c>
+      <c r="I23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>27</v>
+      </c>
+      <c r="F24">
+        <v>18</v>
+      </c>
+      <c r="I24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>27</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" s="27">
+        <v>43862</v>
+      </c>
+      <c r="F35">
+        <v>19</v>
+      </c>
+      <c r="I35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>15</v>
+      </c>
+      <c r="I36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="F44">
+        <v>12</v>
+      </c>
+      <c r="R44">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>13</v>
+      </c>
+      <c r="R45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R47">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5247DA87-7C98-479F-911C-2F3117FE0B00}">
   <dimension ref="A1:G16"/>
   <sheetViews>

</xml_diff>